<commit_message>
added disturbances in p_x for all rule-based scenarios
</commit_message>
<xml_diff>
--- a/EMS_simulation/data_input/hot_water_consumption_artificial_profile_10min_granularity.xlsx
+++ b/EMS_simulation/data_input/hot_water_consumption_artificial_profile_10min_granularity.xlsx
@@ -128,10 +128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B289"/>
+  <dimension ref="A1:B721"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A274" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L289" activeCellId="0" sqref="L289"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A714" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G723" activeCellId="0" sqref="G723"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1260,7 +1260,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
         <v>43221.9652777778</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>24.6666666666667</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
         <v>43221.9722222222</v>
       </c>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
-        <v>43221.9791666667</v>
+        <v>43221.9791666666</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>16</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
-        <v>43221.9861111111</v>
+        <v>43221.986111111</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>19.3333333333333</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
-        <v>43221.9930555556</v>
+        <v>43221.9930555554</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>14.6666666666667</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
-        <v>43222</v>
+        <v>43221.9999999998</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>13.3333333333333</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
-        <v>43222.0069444445</v>
+        <v>43222.0069444441</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>12.6666666666667</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="n">
-        <v>43222.0138888889</v>
+        <v>43222.0138888885</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>11.3333333333333</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="n">
-        <v>43222.0208333334</v>
+        <v>43222.0208333329</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>12</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="n">
-        <v>43222.0277777778</v>
+        <v>43222.0277777773</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>9.33333333333333</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="n">
-        <v>43222.0347222223</v>
+        <v>43222.0347222217</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>10.6666666666667</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="n">
-        <v>43222.0416666667</v>
+        <v>43222.0416666661</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>9</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
-        <v>43222.0486111112</v>
+        <v>43222.0486111105</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>9.33333333333333</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
-        <v>43222.0555555556</v>
+        <v>43222.0555555549</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>7.33333333333333</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
-        <v>43222.0625000001</v>
+        <v>43222.0624999993</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>10.6666666666667</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
-        <v>43222.0694444445</v>
+        <v>43222.0694444437</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>8</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
-        <v>43222.076388889</v>
+        <v>43222.076388888</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>8.33333333333333</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
-        <v>43222.0833333334</v>
+        <v>43222.0833333324</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>4.66666666666667</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="n">
-        <v>43222.0902777779</v>
+        <v>43222.0902777768</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>7.66666666666667</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
-        <v>43222.0972222223</v>
+        <v>43222.0972222212</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>5.33333333333333</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
-        <v>43222.1041666668</v>
+        <v>43222.1041666656</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>4</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
-        <v>43222.1111111112</v>
+        <v>43222.11111111</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>5.66666666666667</v>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
-        <v>43222.1180555557</v>
+        <v>43222.1180555544</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>3.33333333333333</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
-        <v>43222.1250000001</v>
+        <v>43222.1249999988</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>2.66666666666667</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
-        <v>43222.1319444446</v>
+        <v>43222.1319444432</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>3</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
-        <v>43222.138888889</v>
+        <v>43222.1388888876</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>2</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
-        <v>43222.1458333335</v>
+        <v>43222.145833332</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>2.33333333333333</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
-        <v>43222.1527777779</v>
+        <v>43222.1527777763</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>1.33333333333333</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
-        <v>43222.1597222224</v>
+        <v>43222.1597222207</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>0.666666666666667</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
-        <v>43222.1666666668</v>
+        <v>43222.1666666651</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>1.33333333333333</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
-        <v>43222.1736111113</v>
+        <v>43222.1736111095</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>1.66666666666667</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
-        <v>43222.1805555557</v>
+        <v>43222.1805555539</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>3.33333333333333</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
-        <v>43222.1875000002</v>
+        <v>43222.1874999983</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>2.66666666666667</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="n">
-        <v>43222.1944444446</v>
+        <v>43222.1944444427</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>4.66666666666667</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="n">
-        <v>43222.2013888891</v>
+        <v>43222.2013888871</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>6</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
-        <v>43222.2083333335</v>
+        <v>43222.2083333315</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>6.66666666666667</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="n">
-        <v>43222.215277778</v>
+        <v>43222.2152777758</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>10</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="n">
-        <v>43222.2222222224</v>
+        <v>43222.2222222202</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>16.6666666666667</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
-        <v>43222.2291666669</v>
+        <v>43222.2291666646</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>33.3333333333333</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
-        <v>43222.2361111113</v>
+        <v>43222.236111109</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>26.6666666666667</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="n">
-        <v>43222.2430555558</v>
+        <v>43222.2430555534</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>46.6666666666667</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="n">
-        <v>43222.2500000002</v>
+        <v>43222.2499999978</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>53.3333333333333</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="n">
-        <v>43222.2569444447</v>
+        <v>43222.2569444422</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>73.3333333333333</v>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="n">
-        <v>43222.2638888891</v>
+        <v>43222.2638888866</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>76.6666666666667</v>
@@ -1614,7 +1614,7 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
-        <v>43222.2708333336</v>
+        <v>43222.270833331</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>93.3333333333333</v>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
-        <v>43222.277777778</v>
+        <v>43222.2777777753</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>103.333333333333</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
-        <v>43222.2847222225</v>
+        <v>43222.2847222197</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>116.666666666667</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
-        <v>43222.2916666669</v>
+        <v>43222.2916666641</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>120</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
-        <v>43222.2986111114</v>
+        <v>43222.2986111085</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>103.333333333333</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
-        <v>43222.3055555558</v>
+        <v>43222.3055555529</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>93.3333333333333</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
-        <v>43222.3125000003</v>
+        <v>43222.3124999973</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>86.6666666666667</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
-        <v>43222.3194444447</v>
+        <v>43222.3194444417</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>96.6666666666667</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
-        <v>43222.3263888892</v>
+        <v>43222.3263888861</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>100</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
-        <v>43222.3333333336</v>
+        <v>43222.3333333305</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>113.333333333333</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
-        <v>43222.3402777781</v>
+        <v>43222.3402777749</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>100</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
-        <v>43222.3472222225</v>
+        <v>43222.3472222193</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>88.6666666666667</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
-        <v>43222.354166667</v>
+        <v>43222.3541666636</v>
       </c>
       <c r="B197" s="0" t="n">
         <v>65.3333333333333</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="n">
-        <v>43222.3611111114</v>
+        <v>43222.361111108</v>
       </c>
       <c r="B198" s="0" t="n">
         <v>58.6666666666667</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
-        <v>43222.3680555559</v>
+        <v>43222.3680555524</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>44</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
-        <v>43222.3750000003</v>
+        <v>43222.3749999968</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>40</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
-        <v>43222.3819444448</v>
+        <v>43222.3819444412</v>
       </c>
       <c r="B201" s="0" t="n">
         <v>50.6666666666667</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
-        <v>43222.3888888892</v>
+        <v>43222.3888888856</v>
       </c>
       <c r="B202" s="0" t="n">
         <v>52.6666666666667</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
-        <v>43222.3958333337</v>
+        <v>43222.39583333</v>
       </c>
       <c r="B203" s="0" t="n">
         <v>53.3333333333333</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
-        <v>43222.4027777781</v>
+        <v>43222.4027777744</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>60</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
-        <v>43222.4097222226</v>
+        <v>43222.4097222188</v>
       </c>
       <c r="B205" s="0" t="n">
         <v>63.3333333333333</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
-        <v>43222.416666667</v>
+        <v>43222.4166666632</v>
       </c>
       <c r="B206" s="0" t="n">
         <v>66.6666666666667</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
-        <v>43222.4236111115</v>
+        <v>43222.4236111076</v>
       </c>
       <c r="B207" s="0" t="n">
         <v>58</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
-        <v>43222.4305555559</v>
+        <v>43222.4305555519</v>
       </c>
       <c r="B208" s="0" t="n">
         <v>62.6666666666667</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="n">
-        <v>43222.4375000004</v>
+        <v>43222.4374999963</v>
       </c>
       <c r="B209" s="0" t="n">
         <v>57.3333333333333</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
-        <v>43222.4444444448</v>
+        <v>43222.4444444407</v>
       </c>
       <c r="B210" s="0" t="n">
         <v>59.3333333333333</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
-        <v>43222.4513888893</v>
+        <v>43222.4513888851</v>
       </c>
       <c r="B211" s="0" t="n">
         <v>54</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
-        <v>43222.4583333337</v>
+        <v>43222.4583333295</v>
       </c>
       <c r="B212" s="0" t="n">
         <v>53.3333333333333</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
-        <v>43222.4652777782</v>
+        <v>43222.4652777739</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>55.3333333333333</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="n">
-        <v>43222.4722222226</v>
+        <v>43222.4722222183</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>56.6666666666667</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
-        <v>43222.4791666671</v>
+        <v>43222.4791666627</v>
       </c>
       <c r="B215" s="0" t="n">
         <v>58</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="n">
-        <v>43222.4861111115</v>
+        <v>43222.4861111071</v>
       </c>
       <c r="B216" s="0" t="n">
         <v>60.6666666666667</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
-        <v>43222.493055556</v>
+        <v>43222.4930555514</v>
       </c>
       <c r="B217" s="0" t="n">
         <v>61.3333333333333</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
-        <v>43222.5000000004</v>
+        <v>43222.4999999958</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>60</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
-        <v>43222.5069444449</v>
+        <v>43222.5069444402</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>64</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
-        <v>43222.5138888893</v>
+        <v>43222.5138888846</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>52</v>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="n">
-        <v>43222.5208333338</v>
+        <v>43222.520833329</v>
       </c>
       <c r="B221" s="0" t="n">
         <v>54.6666666666667</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="n">
-        <v>43222.5277777782</v>
+        <v>43222.5277777734</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>50.6666666666667</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="n">
-        <v>43222.5347222227</v>
+        <v>43222.5347222178</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>43.3333333333333</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
-        <v>43222.5416666671</v>
+        <v>43222.5416666622</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>46</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
-        <v>43222.5486111116</v>
+        <v>43222.5486111066</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>40.6666666666667</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="n">
-        <v>43222.555555556</v>
+        <v>43222.555555551</v>
       </c>
       <c r="B226" s="0" t="n">
         <v>38.6666666666667</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
-        <v>43222.5625000005</v>
+        <v>43222.5624999953</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>36</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
-        <v>43222.5694444449</v>
+        <v>43222.5694444397</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>36.6666666666667</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
-        <v>43222.5763888894</v>
+        <v>43222.5763888841</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>37.3333333333333</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
-        <v>43222.5833333338</v>
+        <v>43222.5833333285</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>34</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
-        <v>43222.5902777783</v>
+        <v>43222.5902777729</v>
       </c>
       <c r="B231" s="0" t="n">
         <v>38.6666666666667</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
-        <v>43222.5972222227</v>
+        <v>43222.5972222173</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>33.3333333333333</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
-        <v>43222.6041666672</v>
+        <v>43222.6041666617</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>34</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
-        <v>43222.6111111116</v>
+        <v>43222.6111111061</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>38.6666666666667</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
-        <v>43222.6180555561</v>
+        <v>43222.6180555505</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>34</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
-        <v>43222.6250000005</v>
+        <v>43222.6249999949</v>
       </c>
       <c r="B236" s="0" t="n">
         <v>33.3333333333333</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
-        <v>43222.631944445</v>
+        <v>43222.6319444392</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>38</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
-        <v>43222.6388888894</v>
+        <v>43222.6388888836</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>43.3333333333333</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
-        <v>43222.6458333339</v>
+        <v>43222.645833328</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>42</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="n">
-        <v>43222.6527777783</v>
+        <v>43222.6527777724</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>46</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
-        <v>43222.6597222228</v>
+        <v>43222.6597222168</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>46.6666666666667</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
-        <v>43222.6666666672</v>
+        <v>43222.6666666612</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>53.3333333333333</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
-        <v>43222.6736111117</v>
+        <v>43222.6736111056</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>58</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="n">
-        <v>43222.6805555561</v>
+        <v>43222.68055555</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>65.3333333333333</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
-        <v>43222.6875000006</v>
+        <v>43222.6874999944</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>66</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
-        <v>43222.694444445</v>
+        <v>43222.6944444388</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>73.3333333333333</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
-        <v>43222.7013888895</v>
+        <v>43222.7013888832</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>76</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
-        <v>43222.7083333339</v>
+        <v>43222.7083333275</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>79.3333333333333</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="n">
-        <v>43222.7152777784</v>
+        <v>43222.7152777719</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>82</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="n">
-        <v>43222.7222222228</v>
+        <v>43222.7222222163</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>85.3333333333333</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="n">
-        <v>43222.7291666673</v>
+        <v>43222.7291666607</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>88</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="n">
-        <v>43222.7361111117</v>
+        <v>43222.7361111051</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>92.6666666666667</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="n">
-        <v>43222.7430555562</v>
+        <v>43222.7430555495</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>96.6666666666667</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="n">
-        <v>43222.7500000006</v>
+        <v>43222.7499999939</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>94.6666666666667</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="n">
-        <v>43222.7569444451</v>
+        <v>43222.7569444383</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>100.666666666667</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="n">
-        <v>43222.7638888895</v>
+        <v>43222.7638888827</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>97.3333333333333</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="n">
-        <v>43222.770833334</v>
+        <v>43222.770833327</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>104</v>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="n">
-        <v>43222.7777777784</v>
+        <v>43222.7777777714</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>101.333333333333</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="n">
-        <v>43222.7847222229</v>
+        <v>43222.7847222158</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>100</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="n">
-        <v>43222.7916666673</v>
+        <v>43222.7916666602</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>100</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="n">
-        <v>43222.7986111118</v>
+        <v>43222.7986111046</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>96.6666666666667</v>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="n">
-        <v>43222.8055555562</v>
+        <v>43222.805555549</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>90.6666666666667</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="n">
-        <v>43222.8125000007</v>
+        <v>43222.8124999934</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>86.6666666666667</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="n">
-        <v>43222.8194444451</v>
+        <v>43222.8194444378</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>84</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="n">
-        <v>43222.8263888896</v>
+        <v>43222.8263888822</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>81.3333333333333</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="n">
-        <v>43222.833333334</v>
+        <v>43222.8333333266</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>80.6666666666667</v>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="n">
-        <v>43222.8402777785</v>
+        <v>43222.8402777709</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>74.6666666666667</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="n">
-        <v>43222.8472222229</v>
+        <v>43222.8472222153</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>73.3333333333333</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="n">
-        <v>43222.8541666674</v>
+        <v>43222.8541666597</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>88</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="n">
-        <v>43222.8611111118</v>
+        <v>43222.8611111041</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>80.6666666666667</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="n">
-        <v>43222.8680555563</v>
+        <v>43222.8680555485</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>70</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
-        <v>43222.8750000007</v>
+        <v>43222.8749999929</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>73.3333333333333</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
-        <v>43222.8819444452</v>
+        <v>43222.8819444373</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>65.3333333333333</v>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
-        <v>43222.8888888896</v>
+        <v>43222.8888888817</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>58.6666666666667</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="n">
-        <v>43222.8958333341</v>
+        <v>43222.8958333261</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>52</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="n">
-        <v>43222.9027777785</v>
+        <v>43222.9027777705</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>44</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="n">
-        <v>43222.909722223</v>
+        <v>43222.9097222148</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>50.6666666666667</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="n">
-        <v>43222.9166666674</v>
+        <v>43222.9166666592</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>46</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="n">
-        <v>43222.9236111119</v>
+        <v>43222.9236111036</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>36</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="n">
-        <v>43222.9305555563</v>
+        <v>43222.930555548</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>30</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="n">
-        <v>43222.9375000008</v>
+        <v>43222.9374999924</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>22</v>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="n">
-        <v>43222.9444444452</v>
+        <v>43222.9444444368</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>26</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="n">
-        <v>43222.9513888897</v>
+        <v>43222.9513888812</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>19.3333333333333</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="n">
-        <v>43222.9583333341</v>
+        <v>43222.9583333256</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>20</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="n">
-        <v>43222.9652777786</v>
+        <v>43222.96527777</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>24.6666666666667</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="n">
-        <v>43222.972222223</v>
+        <v>43222.9722222144</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>20</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="n">
-        <v>43222.9791666675</v>
+        <v>43222.9791666587</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>16</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="n">
-        <v>43222.9861111119</v>
+        <v>43222.9861111031</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>19.3333333333333</v>
@@ -2446,9 +2446,3465 @@
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="n">
-        <v>43222.9930555564</v>
+        <v>43222.9930555475</v>
       </c>
       <c r="B289" s="0" t="n">
+        <v>14.6666666666667</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="1" t="n">
+        <v>43222.9999999919</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="n">
+        <v>43223.0069444363</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>12.6666666666667</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="n">
+        <v>43223.0138888807</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>11.3333333333333</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="n">
+        <v>43223.0208333251</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="n">
+        <v>43223.0277777695</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="n">
+        <v>43223.0347222139</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="n">
+        <v>43223.0416666583</v>
+      </c>
+      <c r="B296" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="n">
+        <v>43223.0486111026</v>
+      </c>
+      <c r="B297" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="n">
+        <v>43223.055555547</v>
+      </c>
+      <c r="B298" s="0" t="n">
+        <v>7.33333333333333</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="n">
+        <v>43223.0624999914</v>
+      </c>
+      <c r="B299" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="n">
+        <v>43223.0694444358</v>
+      </c>
+      <c r="B300" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="n">
+        <v>43223.0763888802</v>
+      </c>
+      <c r="B301" s="0" t="n">
+        <v>8.33333333333333</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="1" t="n">
+        <v>43223.0833333246</v>
+      </c>
+      <c r="B302" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="n">
+        <v>43223.090277769</v>
+      </c>
+      <c r="B303" s="0" t="n">
+        <v>7.66666666666667</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="1" t="n">
+        <v>43223.0972222134</v>
+      </c>
+      <c r="B304" s="0" t="n">
+        <v>5.33333333333333</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="1" t="n">
+        <v>43223.1041666578</v>
+      </c>
+      <c r="B305" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="1" t="n">
+        <v>43223.1111111022</v>
+      </c>
+      <c r="B306" s="0" t="n">
+        <v>5.66666666666667</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="1" t="n">
+        <v>43223.1180555465</v>
+      </c>
+      <c r="B307" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="1" t="n">
+        <v>43223.1249999909</v>
+      </c>
+      <c r="B308" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="1" t="n">
+        <v>43223.1319444353</v>
+      </c>
+      <c r="B309" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="1" t="n">
+        <v>43223.1388888797</v>
+      </c>
+      <c r="B310" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="1" t="n">
+        <v>43223.1458333241</v>
+      </c>
+      <c r="B311" s="0" t="n">
+        <v>2.33333333333333</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="1" t="n">
+        <v>43223.1527777685</v>
+      </c>
+      <c r="B312" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="1" t="n">
+        <v>43223.1597222129</v>
+      </c>
+      <c r="B313" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="1" t="n">
+        <v>43223.1666666573</v>
+      </c>
+      <c r="B314" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="1" t="n">
+        <v>43223.1736111017</v>
+      </c>
+      <c r="B315" s="0" t="n">
+        <v>1.66666666666667</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="1" t="n">
+        <v>43223.1805555461</v>
+      </c>
+      <c r="B316" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="1" t="n">
+        <v>43223.1874999904</v>
+      </c>
+      <c r="B317" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="1" t="n">
+        <v>43223.1944444348</v>
+      </c>
+      <c r="B318" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="1" t="n">
+        <v>43223.2013888792</v>
+      </c>
+      <c r="B319" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="1" t="n">
+        <v>43223.2083333236</v>
+      </c>
+      <c r="B320" s="0" t="n">
+        <v>6.66666666666667</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="1" t="n">
+        <v>43223.215277768</v>
+      </c>
+      <c r="B321" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="1" t="n">
+        <v>43223.2222222124</v>
+      </c>
+      <c r="B322" s="0" t="n">
+        <v>16.6666666666667</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="1" t="n">
+        <v>43223.2291666568</v>
+      </c>
+      <c r="B323" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="1" t="n">
+        <v>43223.2361111012</v>
+      </c>
+      <c r="B324" s="0" t="n">
+        <v>26.6666666666667</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="1" t="n">
+        <v>43223.2430555456</v>
+      </c>
+      <c r="B325" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="1" t="n">
+        <v>43223.24999999</v>
+      </c>
+      <c r="B326" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="1" t="n">
+        <v>43223.2569444343</v>
+      </c>
+      <c r="B327" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="1" t="n">
+        <v>43223.2638888787</v>
+      </c>
+      <c r="B328" s="0" t="n">
+        <v>76.6666666666667</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="n">
+        <v>43223.2708333231</v>
+      </c>
+      <c r="B329" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="1" t="n">
+        <v>43223.2777777675</v>
+      </c>
+      <c r="B330" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="1" t="n">
+        <v>43223.2847222119</v>
+      </c>
+      <c r="B331" s="0" t="n">
+        <v>116.666666666667</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="1" t="n">
+        <v>43223.2916666563</v>
+      </c>
+      <c r="B332" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="1" t="n">
+        <v>43223.2986111007</v>
+      </c>
+      <c r="B333" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="1" t="n">
+        <v>43223.3055555451</v>
+      </c>
+      <c r="B334" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="1" t="n">
+        <v>43223.3124999895</v>
+      </c>
+      <c r="B335" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="1" t="n">
+        <v>43223.3194444339</v>
+      </c>
+      <c r="B336" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="1" t="n">
+        <v>43223.3263888783</v>
+      </c>
+      <c r="B337" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="n">
+        <v>43223.3333333226</v>
+      </c>
+      <c r="B338" s="0" t="n">
+        <v>113.333333333333</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="1" t="n">
+        <v>43223.340277767</v>
+      </c>
+      <c r="B339" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="1" t="n">
+        <v>43223.3472222114</v>
+      </c>
+      <c r="B340" s="0" t="n">
+        <v>88.6666666666667</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="1" t="n">
+        <v>43223.3541666558</v>
+      </c>
+      <c r="B341" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="1" t="n">
+        <v>43223.3611111002</v>
+      </c>
+      <c r="B342" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="1" t="n">
+        <v>43223.3680555446</v>
+      </c>
+      <c r="B343" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="1" t="n">
+        <v>43223.374999989</v>
+      </c>
+      <c r="B344" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="1" t="n">
+        <v>43223.3819444334</v>
+      </c>
+      <c r="B345" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="1" t="n">
+        <v>43223.3888888778</v>
+      </c>
+      <c r="B346" s="0" t="n">
+        <v>52.6666666666667</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="1" t="n">
+        <v>43223.3958333222</v>
+      </c>
+      <c r="B347" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="1" t="n">
+        <v>43223.4027777665</v>
+      </c>
+      <c r="B348" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="1" t="n">
+        <v>43223.4097222109</v>
+      </c>
+      <c r="B349" s="0" t="n">
+        <v>63.3333333333333</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="1" t="n">
+        <v>43223.4166666553</v>
+      </c>
+      <c r="B350" s="0" t="n">
+        <v>66.6666666666667</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="1" t="n">
+        <v>43223.4236110997</v>
+      </c>
+      <c r="B351" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="1" t="n">
+        <v>43223.4305555441</v>
+      </c>
+      <c r="B352" s="0" t="n">
+        <v>62.6666666666667</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="1" t="n">
+        <v>43223.4374999885</v>
+      </c>
+      <c r="B353" s="0" t="n">
+        <v>57.3333333333333</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="1" t="n">
+        <v>43223.4444444329</v>
+      </c>
+      <c r="B354" s="0" t="n">
+        <v>59.3333333333333</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="1" t="n">
+        <v>43223.4513888773</v>
+      </c>
+      <c r="B355" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="1" t="n">
+        <v>43223.4583333217</v>
+      </c>
+      <c r="B356" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="1" t="n">
+        <v>43223.465277766</v>
+      </c>
+      <c r="B357" s="0" t="n">
+        <v>55.3333333333333</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="1" t="n">
+        <v>43223.4722222104</v>
+      </c>
+      <c r="B358" s="0" t="n">
+        <v>56.6666666666667</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="1" t="n">
+        <v>43223.4791666548</v>
+      </c>
+      <c r="B359" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="1" t="n">
+        <v>43223.4861110992</v>
+      </c>
+      <c r="B360" s="0" t="n">
+        <v>60.6666666666667</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="1" t="n">
+        <v>43223.4930555436</v>
+      </c>
+      <c r="B361" s="0" t="n">
+        <v>61.3333333333333</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="1" t="n">
+        <v>43223.499999988</v>
+      </c>
+      <c r="B362" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="1" t="n">
+        <v>43223.5069444324</v>
+      </c>
+      <c r="B363" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="1" t="n">
+        <v>43223.5138888768</v>
+      </c>
+      <c r="B364" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="1" t="n">
+        <v>43223.5208333212</v>
+      </c>
+      <c r="B365" s="0" t="n">
+        <v>54.6666666666667</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="1" t="n">
+        <v>43223.5277777656</v>
+      </c>
+      <c r="B366" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="1" t="n">
+        <v>43223.5347222099</v>
+      </c>
+      <c r="B367" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="1" t="n">
+        <v>43223.5416666543</v>
+      </c>
+      <c r="B368" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="1" t="n">
+        <v>43223.5486110987</v>
+      </c>
+      <c r="B369" s="0" t="n">
+        <v>40.6666666666667</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="1" t="n">
+        <v>43223.5555555431</v>
+      </c>
+      <c r="B370" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="1" t="n">
+        <v>43223.5624999875</v>
+      </c>
+      <c r="B371" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="1" t="n">
+        <v>43223.5694444319</v>
+      </c>
+      <c r="B372" s="0" t="n">
+        <v>36.6666666666667</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="1" t="n">
+        <v>43223.5763888763</v>
+      </c>
+      <c r="B373" s="0" t="n">
+        <v>37.3333333333333</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="1" t="n">
+        <v>43223.5833333207</v>
+      </c>
+      <c r="B374" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="1" t="n">
+        <v>43223.5902777651</v>
+      </c>
+      <c r="B375" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="1" t="n">
+        <v>43223.5972222095</v>
+      </c>
+      <c r="B376" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="1" t="n">
+        <v>43223.6041666538</v>
+      </c>
+      <c r="B377" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="1" t="n">
+        <v>43223.6111110982</v>
+      </c>
+      <c r="B378" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="1" t="n">
+        <v>43223.6180555426</v>
+      </c>
+      <c r="B379" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="1" t="n">
+        <v>43223.624999987</v>
+      </c>
+      <c r="B380" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="1" t="n">
+        <v>43223.6319444314</v>
+      </c>
+      <c r="B381" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="1" t="n">
+        <v>43223.6388888758</v>
+      </c>
+      <c r="B382" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="1" t="n">
+        <v>43223.6458333202</v>
+      </c>
+      <c r="B383" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="1" t="n">
+        <v>43223.6527777646</v>
+      </c>
+      <c r="B384" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="1" t="n">
+        <v>43223.659722209</v>
+      </c>
+      <c r="B385" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="1" t="n">
+        <v>43223.6666666534</v>
+      </c>
+      <c r="B386" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="1" t="n">
+        <v>43223.6736110977</v>
+      </c>
+      <c r="B387" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="1" t="n">
+        <v>43223.6805555421</v>
+      </c>
+      <c r="B388" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="1" t="n">
+        <v>43223.6874999865</v>
+      </c>
+      <c r="B389" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="1" t="n">
+        <v>43223.6944444309</v>
+      </c>
+      <c r="B390" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="1" t="n">
+        <v>43223.7013888753</v>
+      </c>
+      <c r="B391" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="1" t="n">
+        <v>43223.7083333197</v>
+      </c>
+      <c r="B392" s="0" t="n">
+        <v>79.3333333333333</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="1" t="n">
+        <v>43223.7152777641</v>
+      </c>
+      <c r="B393" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="1" t="n">
+        <v>43223.7222222085</v>
+      </c>
+      <c r="B394" s="0" t="n">
+        <v>85.3333333333333</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="1" t="n">
+        <v>43223.7291666529</v>
+      </c>
+      <c r="B395" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="1" t="n">
+        <v>43223.7361110973</v>
+      </c>
+      <c r="B396" s="0" t="n">
+        <v>92.6666666666667</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="1" t="n">
+        <v>43223.7430555416</v>
+      </c>
+      <c r="B397" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="1" t="n">
+        <v>43223.749999986</v>
+      </c>
+      <c r="B398" s="0" t="n">
+        <v>94.6666666666667</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="1" t="n">
+        <v>43223.7569444304</v>
+      </c>
+      <c r="B399" s="0" t="n">
+        <v>100.666666666667</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="1" t="n">
+        <v>43223.7638888748</v>
+      </c>
+      <c r="B400" s="0" t="n">
+        <v>97.3333333333333</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="1" t="n">
+        <v>43223.7708333192</v>
+      </c>
+      <c r="B401" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="1" t="n">
+        <v>43223.7777777636</v>
+      </c>
+      <c r="B402" s="0" t="n">
+        <v>101.333333333333</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="1" t="n">
+        <v>43223.784722208</v>
+      </c>
+      <c r="B403" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="1" t="n">
+        <v>43223.7916666524</v>
+      </c>
+      <c r="B404" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="1" t="n">
+        <v>43223.7986110968</v>
+      </c>
+      <c r="B405" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="1" t="n">
+        <v>43223.8055555412</v>
+      </c>
+      <c r="B406" s="0" t="n">
+        <v>90.6666666666667</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="1" t="n">
+        <v>43223.8124999855</v>
+      </c>
+      <c r="B407" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="1" t="n">
+        <v>43223.8194444299</v>
+      </c>
+      <c r="B408" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="1" t="n">
+        <v>43223.8263888743</v>
+      </c>
+      <c r="B409" s="0" t="n">
+        <v>81.3333333333333</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="1" t="n">
+        <v>43223.8333333187</v>
+      </c>
+      <c r="B410" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="1" t="n">
+        <v>43223.8402777631</v>
+      </c>
+      <c r="B411" s="0" t="n">
+        <v>74.6666666666667</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="1" t="n">
+        <v>43223.8472222075</v>
+      </c>
+      <c r="B412" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="1" t="n">
+        <v>43223.8541666519</v>
+      </c>
+      <c r="B413" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="1" t="n">
+        <v>43223.8611110963</v>
+      </c>
+      <c r="B414" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="1" t="n">
+        <v>43223.8680555407</v>
+      </c>
+      <c r="B415" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="1" t="n">
+        <v>43223.8749999851</v>
+      </c>
+      <c r="B416" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="1" t="n">
+        <v>43223.8819444294</v>
+      </c>
+      <c r="B417" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="1" t="n">
+        <v>43223.8888888738</v>
+      </c>
+      <c r="B418" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="1" t="n">
+        <v>43223.8958333182</v>
+      </c>
+      <c r="B419" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="1" t="n">
+        <v>43223.9027777626</v>
+      </c>
+      <c r="B420" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="1" t="n">
+        <v>43223.909722207</v>
+      </c>
+      <c r="B421" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="1" t="n">
+        <v>43223.9166666514</v>
+      </c>
+      <c r="B422" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="1" t="n">
+        <v>43223.9236110958</v>
+      </c>
+      <c r="B423" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="1" t="n">
+        <v>43223.9305555402</v>
+      </c>
+      <c r="B424" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="1" t="n">
+        <v>43223.9374999846</v>
+      </c>
+      <c r="B425" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="1" t="n">
+        <v>43223.944444429</v>
+      </c>
+      <c r="B426" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="1" t="n">
+        <v>43223.9513888733</v>
+      </c>
+      <c r="B427" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="1" t="n">
+        <v>43223.9583333177</v>
+      </c>
+      <c r="B428" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="1" t="n">
+        <v>43223.9652777621</v>
+      </c>
+      <c r="B429" s="0" t="n">
+        <v>24.6666666666667</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="1" t="n">
+        <v>43223.9722222065</v>
+      </c>
+      <c r="B430" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="1" t="n">
+        <v>43223.9791666509</v>
+      </c>
+      <c r="B431" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="1" t="n">
+        <v>43223.9861110953</v>
+      </c>
+      <c r="B432" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="1" t="n">
+        <v>43223.9930555397</v>
+      </c>
+      <c r="B433" s="0" t="n">
+        <v>14.6666666666667</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="1" t="n">
+        <v>43223.9999999841</v>
+      </c>
+      <c r="B434" s="0" t="n">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="1" t="n">
+        <v>43224.0069444285</v>
+      </c>
+      <c r="B435" s="0" t="n">
+        <v>12.6666666666667</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="1" t="n">
+        <v>43224.0138888729</v>
+      </c>
+      <c r="B436" s="0" t="n">
+        <v>11.3333333333333</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="1" t="n">
+        <v>43224.0208333172</v>
+      </c>
+      <c r="B437" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="1" t="n">
+        <v>43224.0277777616</v>
+      </c>
+      <c r="B438" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="1" t="n">
+        <v>43224.034722206</v>
+      </c>
+      <c r="B439" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="1" t="n">
+        <v>43224.0416666504</v>
+      </c>
+      <c r="B440" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="1" t="n">
+        <v>43224.0486110948</v>
+      </c>
+      <c r="B441" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="1" t="n">
+        <v>43224.0555555392</v>
+      </c>
+      <c r="B442" s="0" t="n">
+        <v>7.33333333333333</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="1" t="n">
+        <v>43224.0624999836</v>
+      </c>
+      <c r="B443" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="1" t="n">
+        <v>43224.069444428</v>
+      </c>
+      <c r="B444" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="1" t="n">
+        <v>43224.0763888724</v>
+      </c>
+      <c r="B445" s="0" t="n">
+        <v>8.33333333333333</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="1" t="n">
+        <v>43224.0833333168</v>
+      </c>
+      <c r="B446" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="1" t="n">
+        <v>43224.0902777611</v>
+      </c>
+      <c r="B447" s="0" t="n">
+        <v>7.66666666666667</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="1" t="n">
+        <v>43224.0972222055</v>
+      </c>
+      <c r="B448" s="0" t="n">
+        <v>5.33333333333333</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="1" t="n">
+        <v>43224.1041666499</v>
+      </c>
+      <c r="B449" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="1" t="n">
+        <v>43224.1111110943</v>
+      </c>
+      <c r="B450" s="0" t="n">
+        <v>5.66666666666667</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="1" t="n">
+        <v>43224.1180555387</v>
+      </c>
+      <c r="B451" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="1" t="n">
+        <v>43224.1249999831</v>
+      </c>
+      <c r="B452" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="1" t="n">
+        <v>43224.1319444275</v>
+      </c>
+      <c r="B453" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="1" t="n">
+        <v>43224.1388888719</v>
+      </c>
+      <c r="B454" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="1" t="n">
+        <v>43224.1458333163</v>
+      </c>
+      <c r="B455" s="0" t="n">
+        <v>2.33333333333333</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="1" t="n">
+        <v>43224.1527777607</v>
+      </c>
+      <c r="B456" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="1" t="n">
+        <v>43224.159722205</v>
+      </c>
+      <c r="B457" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="1" t="n">
+        <v>43224.1666666494</v>
+      </c>
+      <c r="B458" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="1" t="n">
+        <v>43224.1736110938</v>
+      </c>
+      <c r="B459" s="0" t="n">
+        <v>1.66666666666667</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="1" t="n">
+        <v>43224.1805555382</v>
+      </c>
+      <c r="B460" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="1" t="n">
+        <v>43224.1874999826</v>
+      </c>
+      <c r="B461" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="1" t="n">
+        <v>43224.194444427</v>
+      </c>
+      <c r="B462" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="1" t="n">
+        <v>43224.2013888714</v>
+      </c>
+      <c r="B463" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="1" t="n">
+        <v>43224.2083333158</v>
+      </c>
+      <c r="B464" s="0" t="n">
+        <v>6.66666666666667</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="1" t="n">
+        <v>43224.2152777602</v>
+      </c>
+      <c r="B465" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="1" t="n">
+        <v>43224.2222222046</v>
+      </c>
+      <c r="B466" s="0" t="n">
+        <v>16.6666666666667</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="1" t="n">
+        <v>43224.2291666489</v>
+      </c>
+      <c r="B467" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="1" t="n">
+        <v>43224.2361110933</v>
+      </c>
+      <c r="B468" s="0" t="n">
+        <v>26.6666666666667</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="1" t="n">
+        <v>43224.2430555377</v>
+      </c>
+      <c r="B469" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="1" t="n">
+        <v>43224.2499999821</v>
+      </c>
+      <c r="B470" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="1" t="n">
+        <v>43224.2569444265</v>
+      </c>
+      <c r="B471" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="1" t="n">
+        <v>43224.2638888709</v>
+      </c>
+      <c r="B472" s="0" t="n">
+        <v>76.6666666666667</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="1" t="n">
+        <v>43224.2708333153</v>
+      </c>
+      <c r="B473" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="n">
+        <v>43224.2777777597</v>
+      </c>
+      <c r="B474" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="1" t="n">
+        <v>43224.2847222041</v>
+      </c>
+      <c r="B475" s="0" t="n">
+        <v>116.666666666667</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="1" t="n">
+        <v>43224.2916666485</v>
+      </c>
+      <c r="B476" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="1" t="n">
+        <v>43224.2986110928</v>
+      </c>
+      <c r="B477" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="1" t="n">
+        <v>43224.3055555372</v>
+      </c>
+      <c r="B478" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="n">
+        <v>43224.3124999816</v>
+      </c>
+      <c r="B479" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="n">
+        <v>43224.319444426</v>
+      </c>
+      <c r="B480" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="1" t="n">
+        <v>43224.3263888704</v>
+      </c>
+      <c r="B481" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="1" t="n">
+        <v>43224.3333333148</v>
+      </c>
+      <c r="B482" s="0" t="n">
+        <v>113.333333333333</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="1" t="n">
+        <v>43224.3402777592</v>
+      </c>
+      <c r="B483" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="1" t="n">
+        <v>43224.3472222036</v>
+      </c>
+      <c r="B484" s="0" t="n">
+        <v>88.6666666666667</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="1" t="n">
+        <v>43224.354166648</v>
+      </c>
+      <c r="B485" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="1" t="n">
+        <v>43224.3611110924</v>
+      </c>
+      <c r="B486" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="1" t="n">
+        <v>43224.3680555368</v>
+      </c>
+      <c r="B487" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="1" t="n">
+        <v>43224.3749999811</v>
+      </c>
+      <c r="B488" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="1" t="n">
+        <v>43224.3819444255</v>
+      </c>
+      <c r="B489" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="1" t="n">
+        <v>43224.3888888699</v>
+      </c>
+      <c r="B490" s="0" t="n">
+        <v>52.6666666666667</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="1" t="n">
+        <v>43224.3958333143</v>
+      </c>
+      <c r="B491" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="1" t="n">
+        <v>43224.4027777587</v>
+      </c>
+      <c r="B492" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="1" t="n">
+        <v>43224.4097222031</v>
+      </c>
+      <c r="B493" s="0" t="n">
+        <v>63.3333333333333</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="1" t="n">
+        <v>43224.4166666475</v>
+      </c>
+      <c r="B494" s="0" t="n">
+        <v>66.6666666666667</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="1" t="n">
+        <v>43224.4236110919</v>
+      </c>
+      <c r="B495" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="1" t="n">
+        <v>43224.4305555363</v>
+      </c>
+      <c r="B496" s="0" t="n">
+        <v>62.6666666666667</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="1" t="n">
+        <v>43224.4374999806</v>
+      </c>
+      <c r="B497" s="0" t="n">
+        <v>57.3333333333333</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="1" t="n">
+        <v>43224.444444425</v>
+      </c>
+      <c r="B498" s="0" t="n">
+        <v>59.3333333333333</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="1" t="n">
+        <v>43224.4513888694</v>
+      </c>
+      <c r="B499" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="1" t="n">
+        <v>43224.4583333138</v>
+      </c>
+      <c r="B500" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="1" t="n">
+        <v>43224.4652777582</v>
+      </c>
+      <c r="B501" s="0" t="n">
+        <v>55.3333333333333</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="1" t="n">
+        <v>43224.4722222026</v>
+      </c>
+      <c r="B502" s="0" t="n">
+        <v>56.6666666666667</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="1" t="n">
+        <v>43224.479166647</v>
+      </c>
+      <c r="B503" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="1" t="n">
+        <v>43224.4861110914</v>
+      </c>
+      <c r="B504" s="0" t="n">
+        <v>60.6666666666667</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="1" t="n">
+        <v>43224.4930555358</v>
+      </c>
+      <c r="B505" s="0" t="n">
+        <v>61.3333333333333</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="1" t="n">
+        <v>43224.4999999802</v>
+      </c>
+      <c r="B506" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="1" t="n">
+        <v>43224.5069444245</v>
+      </c>
+      <c r="B507" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="1" t="n">
+        <v>43224.5138888689</v>
+      </c>
+      <c r="B508" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="1" t="n">
+        <v>43224.5208333133</v>
+      </c>
+      <c r="B509" s="0" t="n">
+        <v>54.6666666666667</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="1" t="n">
+        <v>43224.5277777577</v>
+      </c>
+      <c r="B510" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="1" t="n">
+        <v>43224.5347222021</v>
+      </c>
+      <c r="B511" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="1" t="n">
+        <v>43224.5416666465</v>
+      </c>
+      <c r="B512" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A513" s="1" t="n">
+        <v>43224.5486110909</v>
+      </c>
+      <c r="B513" s="0" t="n">
+        <v>40.6666666666667</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A514" s="1" t="n">
+        <v>43224.5555555353</v>
+      </c>
+      <c r="B514" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A515" s="1" t="n">
+        <v>43224.5624999797</v>
+      </c>
+      <c r="B515" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A516" s="1" t="n">
+        <v>43224.5694444241</v>
+      </c>
+      <c r="B516" s="0" t="n">
+        <v>36.6666666666667</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="1" t="n">
+        <v>43224.5763888685</v>
+      </c>
+      <c r="B517" s="0" t="n">
+        <v>37.3333333333333</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A518" s="1" t="n">
+        <v>43224.5833333128</v>
+      </c>
+      <c r="B518" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A519" s="1" t="n">
+        <v>43224.5902777572</v>
+      </c>
+      <c r="B519" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="1" t="n">
+        <v>43224.5972222016</v>
+      </c>
+      <c r="B520" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A521" s="1" t="n">
+        <v>43224.604166646</v>
+      </c>
+      <c r="B521" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A522" s="1" t="n">
+        <v>43224.6111110904</v>
+      </c>
+      <c r="B522" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A523" s="1" t="n">
+        <v>43224.6180555348</v>
+      </c>
+      <c r="B523" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="1" t="n">
+        <v>43224.6249999792</v>
+      </c>
+      <c r="B524" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="1" t="n">
+        <v>43224.6319444236</v>
+      </c>
+      <c r="B525" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A526" s="1" t="n">
+        <v>43224.638888868</v>
+      </c>
+      <c r="B526" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="1" t="n">
+        <v>43224.6458333123</v>
+      </c>
+      <c r="B527" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A528" s="1" t="n">
+        <v>43224.6527777567</v>
+      </c>
+      <c r="B528" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="1" t="n">
+        <v>43224.6597222011</v>
+      </c>
+      <c r="B529" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="1" t="n">
+        <v>43224.6666666455</v>
+      </c>
+      <c r="B530" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="1" t="n">
+        <v>43224.6736110899</v>
+      </c>
+      <c r="B531" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="1" t="n">
+        <v>43224.6805555343</v>
+      </c>
+      <c r="B532" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="1" t="n">
+        <v>43224.6874999787</v>
+      </c>
+      <c r="B533" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="1" t="n">
+        <v>43224.6944444231</v>
+      </c>
+      <c r="B534" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A535" s="1" t="n">
+        <v>43224.7013888675</v>
+      </c>
+      <c r="B535" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A536" s="1" t="n">
+        <v>43224.7083333119</v>
+      </c>
+      <c r="B536" s="0" t="n">
+        <v>79.3333333333333</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="1" t="n">
+        <v>43224.7152777562</v>
+      </c>
+      <c r="B537" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="1" t="n">
+        <v>43224.7222222006</v>
+      </c>
+      <c r="B538" s="0" t="n">
+        <v>85.3333333333333</v>
+      </c>
+    </row>
+    <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="1" t="n">
+        <v>43224.729166645</v>
+      </c>
+      <c r="B539" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="1" t="n">
+        <v>43224.7361110894</v>
+      </c>
+      <c r="B540" s="0" t="n">
+        <v>92.6666666666667</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="1" t="n">
+        <v>43224.7430555338</v>
+      </c>
+      <c r="B541" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="1" t="n">
+        <v>43224.7499999782</v>
+      </c>
+      <c r="B542" s="0" t="n">
+        <v>94.6666666666667</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="1" t="n">
+        <v>43224.7569444226</v>
+      </c>
+      <c r="B543" s="0" t="n">
+        <v>100.666666666667</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="1" t="n">
+        <v>43224.763888867</v>
+      </c>
+      <c r="B544" s="0" t="n">
+        <v>97.3333333333333</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A545" s="1" t="n">
+        <v>43224.7708333114</v>
+      </c>
+      <c r="B545" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A546" s="1" t="n">
+        <v>43224.7777777558</v>
+      </c>
+      <c r="B546" s="0" t="n">
+        <v>101.333333333333</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="1" t="n">
+        <v>43224.7847222001</v>
+      </c>
+      <c r="B547" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="1" t="n">
+        <v>43224.7916666445</v>
+      </c>
+      <c r="B548" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="1" t="n">
+        <v>43224.7986110889</v>
+      </c>
+      <c r="B549" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="1" t="n">
+        <v>43224.8055555333</v>
+      </c>
+      <c r="B550" s="0" t="n">
+        <v>90.6666666666667</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="1" t="n">
+        <v>43224.8124999777</v>
+      </c>
+      <c r="B551" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A552" s="1" t="n">
+        <v>43224.8194444221</v>
+      </c>
+      <c r="B552" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A553" s="1" t="n">
+        <v>43224.8263888665</v>
+      </c>
+      <c r="B553" s="0" t="n">
+        <v>81.3333333333333</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A554" s="1" t="n">
+        <v>43224.8333333109</v>
+      </c>
+      <c r="B554" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A555" s="1" t="n">
+        <v>43224.8402777553</v>
+      </c>
+      <c r="B555" s="0" t="n">
+        <v>74.6666666666667</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="1" t="n">
+        <v>43224.8472221997</v>
+      </c>
+      <c r="B556" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="1" t="n">
+        <v>43224.854166644</v>
+      </c>
+      <c r="B557" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A558" s="1" t="n">
+        <v>43224.8611110884</v>
+      </c>
+      <c r="B558" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A559" s="1" t="n">
+        <v>43224.8680555328</v>
+      </c>
+      <c r="B559" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A560" s="1" t="n">
+        <v>43224.8749999772</v>
+      </c>
+      <c r="B560" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A561" s="1" t="n">
+        <v>43224.8819444216</v>
+      </c>
+      <c r="B561" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A562" s="1" t="n">
+        <v>43224.888888866</v>
+      </c>
+      <c r="B562" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A563" s="1" t="n">
+        <v>43224.8958333104</v>
+      </c>
+      <c r="B563" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A564" s="1" t="n">
+        <v>43224.9027777548</v>
+      </c>
+      <c r="B564" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="1" t="n">
+        <v>43224.9097221992</v>
+      </c>
+      <c r="B565" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A566" s="1" t="n">
+        <v>43224.9166666436</v>
+      </c>
+      <c r="B566" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A567" s="1" t="n">
+        <v>43224.9236110879</v>
+      </c>
+      <c r="B567" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A568" s="1" t="n">
+        <v>43224.9305555323</v>
+      </c>
+      <c r="B568" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A569" s="1" t="n">
+        <v>43224.9374999767</v>
+      </c>
+      <c r="B569" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A570" s="1" t="n">
+        <v>43224.9444444211</v>
+      </c>
+      <c r="B570" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A571" s="1" t="n">
+        <v>43224.9513888655</v>
+      </c>
+      <c r="B571" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A572" s="1" t="n">
+        <v>43224.9583333099</v>
+      </c>
+      <c r="B572" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A573" s="1" t="n">
+        <v>43224.9652777543</v>
+      </c>
+      <c r="B573" s="0" t="n">
+        <v>24.6666666666667</v>
+      </c>
+    </row>
+    <row r="574" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A574" s="1" t="n">
+        <v>43224.9722221987</v>
+      </c>
+      <c r="B574" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A575" s="1" t="n">
+        <v>43224.9791666431</v>
+      </c>
+      <c r="B575" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A576" s="1" t="n">
+        <v>43224.9861110875</v>
+      </c>
+      <c r="B576" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A577" s="1" t="n">
+        <v>43224.9930555318</v>
+      </c>
+      <c r="B577" s="0" t="n">
+        <v>14.6666666666667</v>
+      </c>
+    </row>
+    <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A578" s="1" t="n">
+        <v>43224.9999999762</v>
+      </c>
+      <c r="B578" s="0" t="n">
+        <v>13.3333333333333</v>
+      </c>
+    </row>
+    <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A579" s="1" t="n">
+        <v>43225.0069444206</v>
+      </c>
+      <c r="B579" s="0" t="n">
+        <v>12.6666666666667</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A580" s="1" t="n">
+        <v>43225.013888865</v>
+      </c>
+      <c r="B580" s="0" t="n">
+        <v>11.3333333333333</v>
+      </c>
+    </row>
+    <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A581" s="1" t="n">
+        <v>43225.0208333094</v>
+      </c>
+      <c r="B581" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A582" s="1" t="n">
+        <v>43225.0277777538</v>
+      </c>
+      <c r="B582" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A583" s="1" t="n">
+        <v>43225.0347221982</v>
+      </c>
+      <c r="B583" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A584" s="1" t="n">
+        <v>43225.0416666426</v>
+      </c>
+      <c r="B584" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A585" s="1" t="n">
+        <v>43225.048611087</v>
+      </c>
+      <c r="B585" s="0" t="n">
+        <v>9.33333333333333</v>
+      </c>
+    </row>
+    <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A586" s="1" t="n">
+        <v>43225.0555555314</v>
+      </c>
+      <c r="B586" s="0" t="n">
+        <v>7.33333333333333</v>
+      </c>
+    </row>
+    <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A587" s="1" t="n">
+        <v>43225.0624999757</v>
+      </c>
+      <c r="B587" s="0" t="n">
+        <v>10.6666666666667</v>
+      </c>
+    </row>
+    <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A588" s="1" t="n">
+        <v>43225.0694444201</v>
+      </c>
+      <c r="B588" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A589" s="1" t="n">
+        <v>43225.0763888645</v>
+      </c>
+      <c r="B589" s="0" t="n">
+        <v>8.33333333333333</v>
+      </c>
+    </row>
+    <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A590" s="1" t="n">
+        <v>43225.0833333089</v>
+      </c>
+      <c r="B590" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A591" s="1" t="n">
+        <v>43225.0902777533</v>
+      </c>
+      <c r="B591" s="0" t="n">
+        <v>7.66666666666667</v>
+      </c>
+    </row>
+    <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A592" s="1" t="n">
+        <v>43225.0972221977</v>
+      </c>
+      <c r="B592" s="0" t="n">
+        <v>5.33333333333333</v>
+      </c>
+    </row>
+    <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A593" s="1" t="n">
+        <v>43225.1041666421</v>
+      </c>
+      <c r="B593" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="594" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A594" s="1" t="n">
+        <v>43225.1111110865</v>
+      </c>
+      <c r="B594" s="0" t="n">
+        <v>5.66666666666667</v>
+      </c>
+    </row>
+    <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A595" s="1" t="n">
+        <v>43225.1180555309</v>
+      </c>
+      <c r="B595" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A596" s="1" t="n">
+        <v>43225.1249999753</v>
+      </c>
+      <c r="B596" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A597" s="1" t="n">
+        <v>43225.1319444196</v>
+      </c>
+      <c r="B597" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A598" s="1" t="n">
+        <v>43225.138888864</v>
+      </c>
+      <c r="B598" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A599" s="1" t="n">
+        <v>43225.1458333084</v>
+      </c>
+      <c r="B599" s="0" t="n">
+        <v>2.33333333333333</v>
+      </c>
+    </row>
+    <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A600" s="1" t="n">
+        <v>43225.1527777528</v>
+      </c>
+      <c r="B600" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A601" s="1" t="n">
+        <v>43225.1597221972</v>
+      </c>
+      <c r="B601" s="0" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A602" s="1" t="n">
+        <v>43225.1666666416</v>
+      </c>
+      <c r="B602" s="0" t="n">
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A603" s="1" t="n">
+        <v>43225.173611086</v>
+      </c>
+      <c r="B603" s="0" t="n">
+        <v>1.66666666666667</v>
+      </c>
+    </row>
+    <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A604" s="1" t="n">
+        <v>43225.1805555304</v>
+      </c>
+      <c r="B604" s="0" t="n">
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A605" s="1" t="n">
+        <v>43225.1874999748</v>
+      </c>
+      <c r="B605" s="0" t="n">
+        <v>2.66666666666667</v>
+      </c>
+    </row>
+    <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A606" s="1" t="n">
+        <v>43225.1944444192</v>
+      </c>
+      <c r="B606" s="0" t="n">
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A607" s="1" t="n">
+        <v>43225.2013888635</v>
+      </c>
+      <c r="B607" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A608" s="1" t="n">
+        <v>43225.2083333079</v>
+      </c>
+      <c r="B608" s="0" t="n">
+        <v>6.66666666666667</v>
+      </c>
+    </row>
+    <row r="609" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A609" s="1" t="n">
+        <v>43225.2152777523</v>
+      </c>
+      <c r="B609" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="610" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A610" s="1" t="n">
+        <v>43225.2222221967</v>
+      </c>
+      <c r="B610" s="0" t="n">
+        <v>16.6666666666667</v>
+      </c>
+    </row>
+    <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A611" s="1" t="n">
+        <v>43225.2291666411</v>
+      </c>
+      <c r="B611" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A612" s="1" t="n">
+        <v>43225.2361110855</v>
+      </c>
+      <c r="B612" s="0" t="n">
+        <v>26.6666666666667</v>
+      </c>
+    </row>
+    <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A613" s="1" t="n">
+        <v>43225.2430555299</v>
+      </c>
+      <c r="B613" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A614" s="1" t="n">
+        <v>43225.2499999743</v>
+      </c>
+      <c r="B614" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A615" s="1" t="n">
+        <v>43225.2569444187</v>
+      </c>
+      <c r="B615" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A616" s="1" t="n">
+        <v>43225.2638888631</v>
+      </c>
+      <c r="B616" s="0" t="n">
+        <v>76.6666666666667</v>
+      </c>
+    </row>
+    <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A617" s="1" t="n">
+        <v>43225.2708333074</v>
+      </c>
+      <c r="B617" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A618" s="1" t="n">
+        <v>43225.2777777518</v>
+      </c>
+      <c r="B618" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A619" s="1" t="n">
+        <v>43225.2847221962</v>
+      </c>
+      <c r="B619" s="0" t="n">
+        <v>116.666666666667</v>
+      </c>
+    </row>
+    <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A620" s="1" t="n">
+        <v>43225.2916666406</v>
+      </c>
+      <c r="B620" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A621" s="1" t="n">
+        <v>43225.298611085</v>
+      </c>
+      <c r="B621" s="0" t="n">
+        <v>103.333333333333</v>
+      </c>
+    </row>
+    <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A622" s="1" t="n">
+        <v>43225.3055555294</v>
+      </c>
+      <c r="B622" s="0" t="n">
+        <v>93.3333333333333</v>
+      </c>
+    </row>
+    <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A623" s="1" t="n">
+        <v>43225.3124999738</v>
+      </c>
+      <c r="B623" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A624" s="1" t="n">
+        <v>43225.3194444182</v>
+      </c>
+      <c r="B624" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A625" s="1" t="n">
+        <v>43225.3263888626</v>
+      </c>
+      <c r="B625" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A626" s="1" t="n">
+        <v>43225.333333307</v>
+      </c>
+      <c r="B626" s="0" t="n">
+        <v>113.333333333333</v>
+      </c>
+    </row>
+    <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A627" s="1" t="n">
+        <v>43225.3402777513</v>
+      </c>
+      <c r="B627" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A628" s="1" t="n">
+        <v>43225.3472221957</v>
+      </c>
+      <c r="B628" s="0" t="n">
+        <v>88.6666666666667</v>
+      </c>
+    </row>
+    <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A629" s="1" t="n">
+        <v>43225.3541666401</v>
+      </c>
+      <c r="B629" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A630" s="1" t="n">
+        <v>43225.3611110845</v>
+      </c>
+      <c r="B630" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A631" s="1" t="n">
+        <v>43225.3680555289</v>
+      </c>
+      <c r="B631" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A632" s="1" t="n">
+        <v>43225.3749999733</v>
+      </c>
+      <c r="B632" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A633" s="1" t="n">
+        <v>43225.3819444177</v>
+      </c>
+      <c r="B633" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A634" s="1" t="n">
+        <v>43225.3888888621</v>
+      </c>
+      <c r="B634" s="0" t="n">
+        <v>52.6666666666667</v>
+      </c>
+    </row>
+    <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A635" s="1" t="n">
+        <v>43225.3958333065</v>
+      </c>
+      <c r="B635" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="636" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A636" s="1" t="n">
+        <v>43225.4027777509</v>
+      </c>
+      <c r="B636" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A637" s="1" t="n">
+        <v>43225.4097221952</v>
+      </c>
+      <c r="B637" s="0" t="n">
+        <v>63.3333333333333</v>
+      </c>
+    </row>
+    <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A638" s="1" t="n">
+        <v>43225.4166666396</v>
+      </c>
+      <c r="B638" s="0" t="n">
+        <v>66.6666666666667</v>
+      </c>
+    </row>
+    <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A639" s="1" t="n">
+        <v>43225.423611084</v>
+      </c>
+      <c r="B639" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="640" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A640" s="1" t="n">
+        <v>43225.4305555284</v>
+      </c>
+      <c r="B640" s="0" t="n">
+        <v>62.6666666666667</v>
+      </c>
+    </row>
+    <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A641" s="1" t="n">
+        <v>43225.4374999728</v>
+      </c>
+      <c r="B641" s="0" t="n">
+        <v>57.3333333333333</v>
+      </c>
+    </row>
+    <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A642" s="1" t="n">
+        <v>43225.4444444172</v>
+      </c>
+      <c r="B642" s="0" t="n">
+        <v>59.3333333333333</v>
+      </c>
+    </row>
+    <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="1" t="n">
+        <v>43225.4513888616</v>
+      </c>
+      <c r="B643" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A644" s="1" t="n">
+        <v>43225.458333306</v>
+      </c>
+      <c r="B644" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A645" s="1" t="n">
+        <v>43225.4652777504</v>
+      </c>
+      <c r="B645" s="0" t="n">
+        <v>55.3333333333333</v>
+      </c>
+    </row>
+    <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A646" s="1" t="n">
+        <v>43225.4722221948</v>
+      </c>
+      <c r="B646" s="0" t="n">
+        <v>56.6666666666667</v>
+      </c>
+    </row>
+    <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A647" s="1" t="n">
+        <v>43225.4791666391</v>
+      </c>
+      <c r="B647" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A648" s="1" t="n">
+        <v>43225.4861110835</v>
+      </c>
+      <c r="B648" s="0" t="n">
+        <v>60.6666666666667</v>
+      </c>
+    </row>
+    <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A649" s="1" t="n">
+        <v>43225.4930555279</v>
+      </c>
+      <c r="B649" s="0" t="n">
+        <v>61.3333333333333</v>
+      </c>
+    </row>
+    <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A650" s="1" t="n">
+        <v>43225.4999999723</v>
+      </c>
+      <c r="B650" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A651" s="1" t="n">
+        <v>43225.5069444167</v>
+      </c>
+      <c r="B651" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A652" s="1" t="n">
+        <v>43225.5138888611</v>
+      </c>
+      <c r="B652" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="1" t="n">
+        <v>43225.5208333055</v>
+      </c>
+      <c r="B653" s="0" t="n">
+        <v>54.6666666666667</v>
+      </c>
+    </row>
+    <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A654" s="1" t="n">
+        <v>43225.5277777499</v>
+      </c>
+      <c r="B654" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A655" s="1" t="n">
+        <v>43225.5347221943</v>
+      </c>
+      <c r="B655" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A656" s="1" t="n">
+        <v>43225.5416666387</v>
+      </c>
+      <c r="B656" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A657" s="1" t="n">
+        <v>43225.5486110831</v>
+      </c>
+      <c r="B657" s="0" t="n">
+        <v>40.6666666666667</v>
+      </c>
+    </row>
+    <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A658" s="1" t="n">
+        <v>43225.5555555274</v>
+      </c>
+      <c r="B658" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A659" s="1" t="n">
+        <v>43225.5624999718</v>
+      </c>
+      <c r="B659" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A660" s="1" t="n">
+        <v>43225.5694444162</v>
+      </c>
+      <c r="B660" s="0" t="n">
+        <v>36.6666666666667</v>
+      </c>
+    </row>
+    <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A661" s="1" t="n">
+        <v>43225.5763888606</v>
+      </c>
+      <c r="B661" s="0" t="n">
+        <v>37.3333333333333</v>
+      </c>
+    </row>
+    <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A662" s="1" t="n">
+        <v>43225.583333305</v>
+      </c>
+      <c r="B662" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A663" s="1" t="n">
+        <v>43225.5902777494</v>
+      </c>
+      <c r="B663" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A664" s="1" t="n">
+        <v>43225.5972221938</v>
+      </c>
+      <c r="B664" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A665" s="1" t="n">
+        <v>43225.6041666382</v>
+      </c>
+      <c r="B665" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A666" s="1" t="n">
+        <v>43225.6111110826</v>
+      </c>
+      <c r="B666" s="0" t="n">
+        <v>38.6666666666667</v>
+      </c>
+    </row>
+    <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A667" s="1" t="n">
+        <v>43225.6180555269</v>
+      </c>
+      <c r="B667" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A668" s="1" t="n">
+        <v>43225.6249999713</v>
+      </c>
+      <c r="B668" s="0" t="n">
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A669" s="1" t="n">
+        <v>43225.6319444157</v>
+      </c>
+      <c r="B669" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A670" s="1" t="n">
+        <v>43225.6388888601</v>
+      </c>
+      <c r="B670" s="0" t="n">
+        <v>43.3333333333333</v>
+      </c>
+    </row>
+    <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A671" s="1" t="n">
+        <v>43225.6458333045</v>
+      </c>
+      <c r="B671" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A672" s="1" t="n">
+        <v>43225.6527777489</v>
+      </c>
+      <c r="B672" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A673" s="1" t="n">
+        <v>43225.6597221933</v>
+      </c>
+      <c r="B673" s="0" t="n">
+        <v>46.6666666666667</v>
+      </c>
+    </row>
+    <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A674" s="1" t="n">
+        <v>43225.6666666377</v>
+      </c>
+      <c r="B674" s="0" t="n">
+        <v>53.3333333333333</v>
+      </c>
+    </row>
+    <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A675" s="1" t="n">
+        <v>43225.6736110821</v>
+      </c>
+      <c r="B675" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="1" t="n">
+        <v>43225.6805555265</v>
+      </c>
+      <c r="B676" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A677" s="1" t="n">
+        <v>43225.6874999708</v>
+      </c>
+      <c r="B677" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A678" s="1" t="n">
+        <v>43225.6944444152</v>
+      </c>
+      <c r="B678" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A679" s="1" t="n">
+        <v>43225.7013888596</v>
+      </c>
+      <c r="B679" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A680" s="1" t="n">
+        <v>43225.708333304</v>
+      </c>
+      <c r="B680" s="0" t="n">
+        <v>79.3333333333333</v>
+      </c>
+    </row>
+    <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="1" t="n">
+        <v>43225.7152777484</v>
+      </c>
+      <c r="B681" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="1" t="n">
+        <v>43225.7222221928</v>
+      </c>
+      <c r="B682" s="0" t="n">
+        <v>85.3333333333333</v>
+      </c>
+    </row>
+    <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="1" t="n">
+        <v>43225.7291666372</v>
+      </c>
+      <c r="B683" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="1" t="n">
+        <v>43225.7361110816</v>
+      </c>
+      <c r="B684" s="0" t="n">
+        <v>92.6666666666667</v>
+      </c>
+    </row>
+    <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A685" s="1" t="n">
+        <v>43225.743055526</v>
+      </c>
+      <c r="B685" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A686" s="1" t="n">
+        <v>43225.7499999704</v>
+      </c>
+      <c r="B686" s="0" t="n">
+        <v>94.6666666666667</v>
+      </c>
+    </row>
+    <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A687" s="1" t="n">
+        <v>43225.7569444147</v>
+      </c>
+      <c r="B687" s="0" t="n">
+        <v>100.666666666667</v>
+      </c>
+    </row>
+    <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A688" s="1" t="n">
+        <v>43225.7638888591</v>
+      </c>
+      <c r="B688" s="0" t="n">
+        <v>97.3333333333333</v>
+      </c>
+    </row>
+    <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A689" s="1" t="n">
+        <v>43225.7708333035</v>
+      </c>
+      <c r="B689" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A690" s="1" t="n">
+        <v>43225.7777777479</v>
+      </c>
+      <c r="B690" s="0" t="n">
+        <v>101.333333333333</v>
+      </c>
+    </row>
+    <row r="691" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="1" t="n">
+        <v>43225.7847221923</v>
+      </c>
+      <c r="B691" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A692" s="1" t="n">
+        <v>43225.7916666367</v>
+      </c>
+      <c r="B692" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A693" s="1" t="n">
+        <v>43225.7986110811</v>
+      </c>
+      <c r="B693" s="0" t="n">
+        <v>96.6666666666667</v>
+      </c>
+    </row>
+    <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A694" s="1" t="n">
+        <v>43225.8055555255</v>
+      </c>
+      <c r="B694" s="0" t="n">
+        <v>90.6666666666667</v>
+      </c>
+    </row>
+    <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A695" s="1" t="n">
+        <v>43225.8124999699</v>
+      </c>
+      <c r="B695" s="0" t="n">
+        <v>86.6666666666667</v>
+      </c>
+    </row>
+    <row r="696" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A696" s="1" t="n">
+        <v>43225.8194444143</v>
+      </c>
+      <c r="B696" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A697" s="1" t="n">
+        <v>43225.8263888587</v>
+      </c>
+      <c r="B697" s="0" t="n">
+        <v>81.3333333333333</v>
+      </c>
+    </row>
+    <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A698" s="1" t="n">
+        <v>43225.833333303</v>
+      </c>
+      <c r="B698" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="699" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="1" t="n">
+        <v>43225.8402777474</v>
+      </c>
+      <c r="B699" s="0" t="n">
+        <v>74.6666666666667</v>
+      </c>
+    </row>
+    <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A700" s="1" t="n">
+        <v>43225.8472221918</v>
+      </c>
+      <c r="B700" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A701" s="1" t="n">
+        <v>43225.8541666362</v>
+      </c>
+      <c r="B701" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A702" s="1" t="n">
+        <v>43225.8611110806</v>
+      </c>
+      <c r="B702" s="0" t="n">
+        <v>80.6666666666667</v>
+      </c>
+    </row>
+    <row r="703" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="1" t="n">
+        <v>43225.868055525</v>
+      </c>
+      <c r="B703" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="704" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="1" t="n">
+        <v>43225.8749999694</v>
+      </c>
+      <c r="B704" s="0" t="n">
+        <v>73.3333333333333</v>
+      </c>
+    </row>
+    <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="1" t="n">
+        <v>43225.8819444138</v>
+      </c>
+      <c r="B705" s="0" t="n">
+        <v>65.3333333333333</v>
+      </c>
+    </row>
+    <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A706" s="1" t="n">
+        <v>43225.8888888582</v>
+      </c>
+      <c r="B706" s="0" t="n">
+        <v>58.6666666666667</v>
+      </c>
+    </row>
+    <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A707" s="1" t="n">
+        <v>43225.8958333025</v>
+      </c>
+      <c r="B707" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="708" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A708" s="1" t="n">
+        <v>43225.9027777469</v>
+      </c>
+      <c r="B708" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A709" s="1" t="n">
+        <v>43225.9097221913</v>
+      </c>
+      <c r="B709" s="0" t="n">
+        <v>50.6666666666667</v>
+      </c>
+    </row>
+    <row r="710" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A710" s="1" t="n">
+        <v>43225.9166666357</v>
+      </c>
+      <c r="B710" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="711" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A711" s="1" t="n">
+        <v>43225.9236110801</v>
+      </c>
+      <c r="B711" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="712" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A712" s="1" t="n">
+        <v>43225.9305555245</v>
+      </c>
+      <c r="B712" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="713" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A713" s="1" t="n">
+        <v>43225.9374999689</v>
+      </c>
+      <c r="B713" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="714" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A714" s="1" t="n">
+        <v>43225.9444444133</v>
+      </c>
+      <c r="B714" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="715" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="1" t="n">
+        <v>43225.9513888577</v>
+      </c>
+      <c r="B715" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="716" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A716" s="1" t="n">
+        <v>43225.9583333021</v>
+      </c>
+      <c r="B716" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="717" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A717" s="1" t="n">
+        <v>43225.9652777464</v>
+      </c>
+      <c r="B717" s="0" t="n">
+        <v>24.6666666666667</v>
+      </c>
+    </row>
+    <row r="718" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="1" t="n">
+        <v>43225.9722221908</v>
+      </c>
+      <c r="B718" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="719" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A719" s="1" t="n">
+        <v>43225.9791666352</v>
+      </c>
+      <c r="B719" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="720" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A720" s="1" t="n">
+        <v>43225.9861110796</v>
+      </c>
+      <c r="B720" s="0" t="n">
+        <v>19.3333333333333</v>
+      </c>
+    </row>
+    <row r="721" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A721" s="1" t="n">
+        <v>43225.993055524</v>
+      </c>
+      <c r="B721" s="0" t="n">
         <v>14.6666666666667</v>
       </c>
     </row>

</xml_diff>